<commit_message>
finished cnn with pytorch
</commit_message>
<xml_diff>
--- a/f-file/datamark.xlsx
+++ b/f-file/datamark.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/Repos/graduate-dissertation/f-file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4E5249-15F6-DE4F-99E2-E414BFAB5350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44A3E1C-FC0B-DA45-B109-58D0A8FADCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="17440" xr2:uid="{E3E7DDD0-A658-F947-8E38-D6233F66BE77}"/>
+    <workbookView xWindow="480" yWindow="780" windowWidth="15120" windowHeight="17440" xr2:uid="{E3E7DDD0-A658-F947-8E38-D6233F66BE77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$25</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="17">
   <si>
     <t>temperature</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +82,30 @@
   </si>
   <si>
     <t>IsTrain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺少md</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>md飞了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15026 frames</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10490 frames</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -147,9 +174,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +214,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -293,7 +320,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,7 +462,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -443,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D329DE-26B5-8A4F-A5C0-9DF9AA35A8EC}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -456,7 +483,7 @@
     <col min="3" max="3" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -472,8 +499,11 @@
       <c r="E1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -489,8 +519,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -504,10 +537,13 @@
         <v>1.0760000000000001</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -523,8 +559,11 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -540,8 +579,11 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -557,8 +599,14 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -572,10 +620,13 @@
         <v>23.555</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -591,8 +642,14 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -608,8 +665,11 @@
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -623,10 +683,13 @@
         <v>0.63300000000000001</v>
       </c>
       <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -642,8 +705,11 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -657,10 +723,13 @@
         <v>4.8220000000000001</v>
       </c>
       <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -676,8 +745,11 @@
       <c r="E13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -691,10 +763,13 @@
         <v>0.25</v>
       </c>
       <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -710,8 +785,11 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -725,10 +803,13 @@
         <v>2.1659999999999999</v>
       </c>
       <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -744,8 +825,11 @@
       <c r="E17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -761,8 +845,11 @@
       <c r="E18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -776,10 +863,13 @@
         <v>2.1459999999999999</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -795,8 +885,11 @@
       <c r="E20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -812,8 +905,11 @@
       <c r="E21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -829,8 +925,11 @@
       <c r="E22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -846,8 +945,11 @@
       <c r="E23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -863,8 +965,11 @@
       <c r="E24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -880,9 +985,14 @@
       <c r="E25">
         <v>1</v>
       </c>
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F25" xr:uid="{45D329DE-26B5-8A4F-A5C0-9DF9AA35A8EC}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>